<commit_message>
change file name of personalizer
</commit_message>
<xml_diff>
--- a/filesToCheckPersonalizer.xlsx
+++ b/filesToCheckPersonalizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-avinashbb\gitCloneCheck\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E6B458-4D54-42E8-A6C6-A8F027E15DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022A54F7-CCB9-440E-9A8F-734DC6684D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalizerItems" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
   <si>
     <t>url</t>
   </si>
@@ -66,6 +66,57 @@
   </si>
   <si>
     <t>https://www.microsoft.com/en-sg/store/b/accessories</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/ja-jp/store/b/accessories</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us</t>
+  </si>
+  <si>
+    <t>29225</t>
+  </si>
+  <si>
+    <t>section[id*='content-card'] .col</t>
+  </si>
+  <si>
+    <t>0.2,0.3,0.5</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/store/collections/certifiedrefurbished</t>
+  </si>
+  <si>
+    <t>26945</t>
+  </si>
+  <si>
+    <t>.expAPItem</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/store/collections/surfacelist</t>
+  </si>
+  <si>
+    <t>28806A</t>
+  </si>
+  <si>
+    <t>.wrapper-28806A .col</t>
+  </si>
+  <si>
+    <t>28806B</t>
+  </si>
+  <si>
+    <t>.wrapper-28806B .col</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/store/collections/microsoftsurfacedeals</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/store/collections/allsurfaceaccessories</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/store/collections/businessdevices</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/store/collections/certifiedrefurbishedsurface</t>
   </si>
   <si>
     <t>exp_id</t>
@@ -556,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -690,10 +741,214 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E7" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E1 A3:E19 A2:B2 D2:E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -702,7 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F286830-D7E2-478C-B68D-A5E2F78EF58A}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -718,395 +973,395 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>23619</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>23619</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>23619</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>23619</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>23619</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <v>23619</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>23619</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>23619</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>23619</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>23619</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B12">
         <v>23619</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>23619</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B14">
         <v>23619</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>23619</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B16">
         <v>23619</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <v>23619</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B18">
         <v>23619</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>23619</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>23619</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>23619</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>23619</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B23">
         <v>23619</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>23619</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>23619</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>23619</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>23619</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>23619</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B29">
         <v>23619</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B30">
         <v>23619</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B31">
         <v>23619</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B32">
         <v>23619</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B33">
         <v>23619</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B34">
         <v>23619</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B35">
         <v>23619</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B36">
         <v>23619</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made some changes in consoleError js realted to reading issue
</commit_message>
<xml_diff>
--- a/filesToCheckPersonalizer.xlsx
+++ b/filesToCheckPersonalizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-avinashbb\gitCloneCheck\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022A54F7-CCB9-440E-9A8F-734DC6684D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8B6247-B112-49B3-B8F0-1C92D953CF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
   <si>
     <t>url</t>
   </si>
@@ -607,13 +607,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="60.4140625" customWidth="1"/>
     <col min="2" max="2" width="12.9140625" customWidth="1"/>
@@ -622,7 +622,7 @@
     <col min="5" max="5" width="15.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -741,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -775,7 +775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -826,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -928,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -942,13 +942,30 @@
         <v>8</v>
       </c>
       <c r="E19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A3:E19 A2:B2 D2:E2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E20" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>